<commit_message>
more console logs added
</commit_message>
<xml_diff>
--- a/usedData/Reports.xlsx
+++ b/usedData/Reports.xlsx
@@ -511,25 +511,25 @@
         <v>0xE08dB007b15905d64412efd4127705cCd3211062</v>
       </c>
       <c r="C2" t="str">
-        <v>0xB8A49cC4476c53eBdaA8132f912921fF3c61dCCB</v>
+        <v>0xdE4bBfF9ea4274d5d367713D6cE89E0C72A34FbB</v>
       </c>
       <c r="D2">
-        <v>766</v>
+        <v>657</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>678</v>
+        <v>754</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1381</v>
+        <v>1158</v>
       </c>
       <c r="I2" t="str">
-        <v>044716</v>
+        <v>044704</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -567,25 +567,25 @@
         <v>0x43B3770794deC6f97F0DEF8B343e18603b71916D</v>
       </c>
       <c r="C3" t="str">
-        <v>0x5050C1F21E91A02b843bfE6a079754d30133746C</v>
+        <v>0xdE126326483911F550447ee90389354451362d44</v>
       </c>
       <c r="D3">
-        <v>757</v>
+        <v>632</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>822</v>
+        <v>771</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>1405</v>
+        <v>1439</v>
       </c>
       <c r="I3" t="str">
-        <v>044716</v>
+        <v>044704</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -623,22 +623,22 @@
         <v>0x2804b8FfD21b18292797b0fc533A1769B701582E</v>
       </c>
       <c r="C4" t="str">
-        <v>0xf749D316B4F6Af0490e0Ceb977229b3cDd748436</v>
+        <v>0xa674cbe30032Cfc52e88251d9B41cDb1Ac5E74BB</v>
       </c>
       <c r="D4">
-        <v>602</v>
+        <v>641</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>914</v>
+        <v>672</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>1337</v>
+        <v>1365</v>
       </c>
       <c r="I4" t="str">
         <v>044716</v>
@@ -679,22 +679,22 @@
         <v>0x12c814Cbd2AbB4275981022F610779E439A44808</v>
       </c>
       <c r="C5" t="str">
-        <v>0x1Aa57a3830041613fe02CEBc46a2cEBD798d8548</v>
+        <v>0x213b30Cd94aB7bEC9042a5aa631ad829F93c4F40</v>
       </c>
       <c r="D5">
-        <v>624</v>
+        <v>754</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>818</v>
+        <v>978</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1653</v>
+        <v>1204</v>
       </c>
       <c r="I5" t="str">
         <v>044716</v>
@@ -735,22 +735,22 @@
         <v>0x5a0fb59F2c4323d36e3fEaFFE4E0d017e501185F</v>
       </c>
       <c r="C6" t="str">
-        <v>0x6CAaf72491C5e34e0de7F51c1AFf43e47b55CF70</v>
+        <v>0x4798D35C6F5e3f063e320d0D4400bF3B5c161142</v>
       </c>
       <c r="D6">
-        <v>716</v>
+        <v>599</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>724</v>
+        <v>841</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1427</v>
+        <v>1472</v>
       </c>
       <c r="I6" t="str">
         <v>044716</v>
@@ -791,25 +791,25 @@
         <v>0x741B537e1301B7b8dd1dDC5Cd6729307bc7b933A</v>
       </c>
       <c r="C7" t="str">
-        <v>0x1b7d1dAbb37a5606503eD25668fD296Cd566cC61</v>
+        <v>0x6e3b29b1bEbE573c5e1B0B7575e12F0C5E2B2E92</v>
       </c>
       <c r="D7">
-        <v>612</v>
+        <v>626</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>899</v>
+        <v>771</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1557</v>
+        <v>1120</v>
       </c>
       <c r="I7" t="str">
-        <v>044716</v>
+        <v>044704</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -847,22 +847,22 @@
         <v>0x5CA90C91c3D51a6B9B24A2894baf715977A63b8f</v>
       </c>
       <c r="C8" t="str">
-        <v>0x75C3bc1377eE105cd98822Bb7fbb9C206D98983d</v>
+        <v>0x8Ba1Ee5d38dBEB24B34468310b0099De1D80A438</v>
       </c>
       <c r="S8">
-        <v>2578</v>
+        <v>3961</v>
       </c>
       <c r="T8">
         <v>0</v>
       </c>
       <c r="U8" t="str">
-        <v>012397821224782</v>
+        <v>0123978212247821224782</v>
       </c>
       <c r="V8">
         <v>0</v>
       </c>
       <c r="W8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X8">
         <v>0</v>
@@ -876,16 +876,16 @@
         <v>0x37c5d74877e1579e59F2E05F2768e3Ffa09aE086</v>
       </c>
       <c r="C9" t="str">
-        <v>0x5609394A9eDCe2aA12a479B9Ac362919eBcaB1C1</v>
+        <v>0x5F05cD22c404690DB975b939eA303409F03C8393</v>
       </c>
       <c r="S9">
-        <v>1623</v>
+        <v>1255</v>
       </c>
       <c r="T9">
         <v>0</v>
       </c>
       <c r="U9" t="str">
-        <v>01239782</v>
+        <v>01239770</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -905,22 +905,22 @@
         <v>0x94d53aA0c00aB27bA27fEeCbA033E2D373465673</v>
       </c>
       <c r="C10" t="str">
-        <v>0xC18399717f4CF8092EF0C9FAdE66Ae83884Ca6E2</v>
+        <v>0xba542c0b1731bdd33A3a51Fa0523e329052F4782</v>
       </c>
       <c r="S10">
-        <v>4969</v>
+        <v>2500</v>
       </c>
       <c r="T10">
         <v>0</v>
       </c>
       <c r="U10" t="str">
-        <v>0123978212247821224782</v>
+        <v>012397701224782</v>
       </c>
       <c r="V10">
         <v>0</v>
       </c>
       <c r="W10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X10">
         <v>0</v>
@@ -934,16 +934,16 @@
         <v>0x1Aad5cc36C8da871AD28eE20fa923972d9D0e354</v>
       </c>
       <c r="C11" t="str">
-        <v>0xE8C64C69Fd19446D01d39650277a216a09E3d999</v>
+        <v>0x039F1AaCd0Aa6652f5897a32452c0e2B5b471862</v>
       </c>
       <c r="Y11">
-        <v>6330</v>
+        <v>5200</v>
       </c>
       <c r="Z11">
-        <v>4459</v>
+        <v>4852</v>
       </c>
       <c r="AA11">
-        <v>4594</v>
+        <v>4344</v>
       </c>
       <c r="AB11" t="str">
         <v>01097919479194791947919479194791</v>

</xml_diff>